<commit_message>
Added the file and sample metadata for the flow cytometry experiment
</commit_message>
<xml_diff>
--- a/config/order/manual_l3.xlsx
+++ b/config/order/manual_l3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t>CD4 naive</t>
   </si>
@@ -109,6 +109,120 @@
   </si>
   <si>
     <t>B memory</t>
+  </si>
+  <si>
+    <t>Lin-</t>
+  </si>
+  <si>
+    <t>Multiplet</t>
+  </si>
+  <si>
+    <t>CD8 CTL</t>
+  </si>
+  <si>
+    <t>Intermediate monocyte</t>
+  </si>
+  <si>
+    <t>Celltype</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>#7FC97F</t>
+  </si>
+  <si>
+    <t>#BEAED4</t>
+  </si>
+  <si>
+    <t>#FDC086</t>
+  </si>
+  <si>
+    <t>#FFFF99</t>
+  </si>
+  <si>
+    <t>#386CB0</t>
+  </si>
+  <si>
+    <t>#F0027F</t>
+  </si>
+  <si>
+    <t>#BF5B17</t>
+  </si>
+  <si>
+    <t>#666666</t>
+  </si>
+  <si>
+    <t>#1B9E77</t>
+  </si>
+  <si>
+    <t>#D95F02</t>
+  </si>
+  <si>
+    <t>#7570B3</t>
+  </si>
+  <si>
+    <t>#E7298A</t>
+  </si>
+  <si>
+    <t>#66A61E</t>
+  </si>
+  <si>
+    <t>#E6AB02</t>
+  </si>
+  <si>
+    <t>#A6761D</t>
+  </si>
+  <si>
+    <t>#A6CEE3</t>
+  </si>
+  <si>
+    <t>#1F78B4</t>
+  </si>
+  <si>
+    <t>#B2DF8A</t>
+  </si>
+  <si>
+    <t>#33A02C</t>
+  </si>
+  <si>
+    <t>#FB9A99</t>
+  </si>
+  <si>
+    <t>#E31A1C</t>
+  </si>
+  <si>
+    <t>#FDBF6F</t>
+  </si>
+  <si>
+    <t>#FF7F00</t>
+  </si>
+  <si>
+    <t>#CAB2D6</t>
+  </si>
+  <si>
+    <t>#6A3D9A</t>
+  </si>
+  <si>
+    <t>#B15928</t>
+  </si>
+  <si>
+    <t>#FBB4AE</t>
+  </si>
+  <si>
+    <t>#B3CDE3</t>
+  </si>
+  <si>
+    <t>#CCEBC5</t>
+  </si>
+  <si>
+    <t>#DECBE4</t>
+  </si>
+  <si>
+    <t>#FED9A6</t>
+  </si>
+  <si>
+    <t>#FFFFCC</t>
   </si>
 </sst>
 </file>
@@ -915,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F1:F30"/>
+  <dimension ref="F1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +1042,7 @@
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
@@ -948,154 +1062,284 @@
     <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F16" t="s">
+      <c r="G17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" t="s">
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
+      <c r="G19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" t="s">
+      <c r="G20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" t="s">
+      <c r="G22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
+      <c r="G23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" t="s">
+      <c r="G24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
+      <c r="G26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" t="s">
+      <c r="G27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26" t="s">
+      <c r="G28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F27" t="s">
+      <c r="G29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
+      <c r="G30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
+      <c r="G31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
+      <c r="G32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
         <v>8</v>
+      </c>
+      <c r="G35" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final version prior to submission
</commit_message>
<xml_diff>
--- a/config/order/manual_l3.xlsx
+++ b/config/order/manual_l3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\basic\divg\kgres\projects\PRJ0000008_EPICCD\anti_a4b7_sc\src\snakemake\config\order\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\basic\divg\kgres\projects\PRJ0000008_EPICCD\anti_a4b7_sc\config\order\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>CD4 naive</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>#FFFFCC</t>
+  </si>
+  <si>
+    <t>#E5D8BD</t>
   </si>
 </sst>
 </file>
@@ -1029,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F1:G35"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,283 +1065,283 @@
     <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="B2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
+      <c r="B3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
+      <c r="B4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" t="s">
+      <c r="B5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" t="s">
+      <c r="B6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" t="s">
+      <c r="B7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="G8" t="s">
+      <c r="B8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="G9" t="s">
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F15" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F18" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="G18" t="s">
+      <c r="B18" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F19" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="G19" t="s">
+      <c r="B19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="G20" t="s">
+      <c r="B20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F21" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="G21" t="s">
+      <c r="B21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="G22" t="s">
+      <c r="B22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F23" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="G23" t="s">
+      <c r="B23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>3</v>
       </c>
-      <c r="G24" t="s">
+      <c r="B24" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F25" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>33</v>
       </c>
-      <c r="G25" t="s">
+      <c r="B25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F26" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>11</v>
       </c>
-      <c r="G26" t="s">
+      <c r="B26" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F27" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="G27" t="s">
+      <c r="B27" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>12</v>
       </c>
-      <c r="G28" t="s">
+      <c r="B28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>14</v>
       </c>
-      <c r="G29" t="s">
+      <c r="B29" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>19</v>
       </c>
-      <c r="G30" t="s">
+      <c r="B30" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>6</v>
       </c>
-      <c r="G31" t="s">
+      <c r="B31" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>23</v>
       </c>
-      <c r="G32" t="s">
+      <c r="B32" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F33" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
-      <c r="G33" t="s">
+      <c r="B33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F34" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>31</v>
       </c>
-      <c r="G34" t="s">
+      <c r="B34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F35" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>8</v>
       </c>
-      <c r="G35" t="s">
+      <c r="B35" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>